<commit_message>
Get-Answers updated with interface mappings.
</commit_message>
<xml_diff>
--- a/FPOD_Build_Worksheet.xlsx
+++ b/FPOD_Build_Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="28770" windowHeight="9600" tabRatio="845" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="28770" windowHeight="9600" tabRatio="845"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="8" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="iSCSI Variables" sheetId="12" state="hidden" r:id="rId10"/>
     <sheet name="Answers" sheetId="10" state="hidden" r:id="rId11"/>
     <sheet name="hidden work" sheetId="9" state="hidden" r:id="rId12"/>
-    <sheet name="Interface map" sheetId="16" r:id="rId13"/>
+    <sheet name="Interface map" sheetId="16" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="Cisco_Nexus_1110_X_A">Interfaces!$A$76:$E$77</definedName>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="1097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="1089">
   <si>
     <t>UCSM Mgmt VIP</t>
   </si>
@@ -3189,42 +3189,6 @@
     <t>&lt;&lt;Nexus_B&gt;&gt;</t>
   </si>
   <si>
-    <t>NetApp_B</t>
-  </si>
-  <si>
-    <t>NetApp_A</t>
-  </si>
-  <si>
-    <t>NetApp_B_Cluster</t>
-  </si>
-  <si>
-    <t>NetApp_A_Cluster</t>
-  </si>
-  <si>
-    <t>Nexus_B_1</t>
-  </si>
-  <si>
-    <t>Nexus_B_2</t>
-  </si>
-  <si>
-    <t>Fabric_Interconnect_A</t>
-  </si>
-  <si>
-    <t>Fabric_Interconnect_A_FAB_A1</t>
-  </si>
-  <si>
-    <t>Fabric_Interconnect_A_FAB_A2</t>
-  </si>
-  <si>
-    <t>Fabric_Interconnect_B</t>
-  </si>
-  <si>
-    <t>Fabric_Interconnect_B_FAB_B1</t>
-  </si>
-  <si>
-    <t>Fabric_Interconnect_B_FAB_B2</t>
-  </si>
-  <si>
     <t>&lt;&lt;NetApp_A&gt;&gt;</t>
   </si>
   <si>
@@ -3234,91 +3198,19 @@
     <t>Nexus 5548 B (cluster)</t>
   </si>
   <si>
-    <t>Nexus_B_cluster</t>
-  </si>
-  <si>
-    <t>Nexus_A_cluster</t>
-  </si>
-  <si>
-    <t>NetApp_B_2</t>
-  </si>
-  <si>
-    <t>NetApp_B_1</t>
-  </si>
-  <si>
-    <t>SAS</t>
-  </si>
-  <si>
-    <t>gbe_management</t>
-  </si>
-  <si>
-    <t>Nexus_B</t>
-  </si>
-  <si>
-    <t>Nexus_A</t>
-  </si>
-  <si>
     <t>&lt;&lt;NetApp_B&gt;&gt;</t>
   </si>
   <si>
-    <t>NetApp_A_1</t>
-  </si>
-  <si>
-    <t>NetApp_A_2</t>
-  </si>
-  <si>
     <t>&lt;&lt;Fabric_Interconnect_A&gt;&gt;</t>
   </si>
   <si>
-    <t>Chassis_1_FEXA_1</t>
-  </si>
-  <si>
-    <t>Chassis_1_FEXA_4</t>
-  </si>
-  <si>
-    <t>Chassis_1_FEXA_3</t>
-  </si>
-  <si>
-    <t>Chassis_1_FEXA_2</t>
-  </si>
-  <si>
-    <t>Nexus_A_FAB_A_1</t>
-  </si>
-  <si>
-    <t>Nexus_A_FAB_A_2</t>
-  </si>
-  <si>
     <t>&lt;&lt;Fabric_Interconnect_B&gt;&gt;</t>
   </si>
   <si>
-    <t>Chassis_1_FEXB_1</t>
-  </si>
-  <si>
-    <t>Chassis_1_FEXB_2</t>
-  </si>
-  <si>
-    <t>Chassis_1_FEXB_3</t>
-  </si>
-  <si>
-    <t>Chassis_1_FEXB_4</t>
-  </si>
-  <si>
-    <t>Nexus_A_FAB_B_1</t>
-  </si>
-  <si>
-    <t>Nexus_A_FAB_B_2</t>
-  </si>
-  <si>
     <t>&lt;&lt;1000v_A&gt;&gt;</t>
   </si>
   <si>
     <t>&lt;&lt;1000v_B&gt;&gt;</t>
-  </si>
-  <si>
-    <t>1000v_B</t>
-  </si>
-  <si>
-    <t>1000v_A</t>
   </si>
   <si>
     <r>
@@ -3655,6 +3547,90 @@
       </rPr>
       <t xml:space="preserve"> (4)</t>
     </r>
+  </si>
+  <si>
+    <t>&lt;&lt;NetApp_A_Cluster&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;NetApp_B_Cluster&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Nexus_B_1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Nexus_B_2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Fabric_Interconnect_A_FAB_A1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Fabric_Interconnect_A_FAB_A2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Fabric_Interconnect_B_FAB_B1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Fabric_Interconnect_B_FAB_B2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;gbe_management&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;NetApp_B_1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;NetApp_B_2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;SAS&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Nexus_A_cluster&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Nexus_B_cluster&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;NetApp_A_1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;NetApp_A_2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Chassis_1_FEXA_1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Chassis_1_FEXA_2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Chassis_1_FEXA_3&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Chassis_1_FEXA_4&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Nexus_A_FAB_A_1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Nexus_A_FAB_A_2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Chassis_1_FEXB_1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Chassis_1_FEXB_2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Chassis_1_FEXB_3&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Chassis_1_FEXB_4&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Nexus_A_FAB_B_1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Nexus_A_FAB_B_2&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -4707,7 +4683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -8469,8 +8445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8485,7 +8461,7 @@
         <v>1027</v>
       </c>
       <c r="B2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP("NetApp Controller A",Nexus_5548_A,2,FALSE)</f>
@@ -8497,7 +8473,7 @@
         <v>1027</v>
       </c>
       <c r="B3" t="s">
-        <v>1029</v>
+        <v>1032</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP("NetApp Controller B",Nexus_5548_A,2,FALSE)</f>
@@ -8509,7 +8485,7 @@
         <v>1027</v>
       </c>
       <c r="B4" t="s">
-        <v>1032</v>
+        <v>1061</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP("NetApp Controller A (cluster)",Nexus_5548_A,2,FALSE)</f>
@@ -8521,7 +8497,7 @@
         <v>1027</v>
       </c>
       <c r="B5" t="s">
-        <v>1031</v>
+        <v>1062</v>
       </c>
       <c r="C5" t="str">
         <f>VLOOKUP("NetApp Controller B (cluster)",Nexus_5548_A,2,FALSE)</f>
@@ -8533,7 +8509,7 @@
         <v>1027</v>
       </c>
       <c r="B6" t="s">
-        <v>1033</v>
+        <v>1063</v>
       </c>
       <c r="C6" t="str">
         <f>VLOOKUP("Cisco Nexus 5548 B (1)",Nexus_5548_A,2,FALSE)</f>
@@ -8545,7 +8521,7 @@
         <v>1027</v>
       </c>
       <c r="B7" t="s">
-        <v>1034</v>
+        <v>1064</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP("Cisco Nexus 5548 B (2)",Nexus_5548_A,2,FALSE)</f>
@@ -8557,7 +8533,7 @@
         <v>1027</v>
       </c>
       <c r="B8" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C8" t="str">
         <f>VLOOKUP("Cisco UCS Fabric Interconnect A",Nexus_5548_A,2,FALSE)</f>
@@ -8569,7 +8545,7 @@
         <v>1027</v>
       </c>
       <c r="B9" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP("Cisco UCS Fabric Interconnect B",Nexus_5548_A,2,FALSE)</f>
@@ -8581,7 +8557,7 @@
         <v>1027</v>
       </c>
       <c r="B10" t="s">
-        <v>1036</v>
+        <v>1065</v>
       </c>
       <c r="C10" t="str">
         <f>VLOOKUP("Cisco UCS Fabric Interconnect A (FAB A1)",Nexus_5548_A,2,FALSE)</f>
@@ -8593,7 +8569,7 @@
         <v>1027</v>
       </c>
       <c r="B11" t="s">
-        <v>1037</v>
+        <v>1066</v>
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP("Cisco UCS Fabric Interconnect A (FAB A2)",Nexus_5548_A,2,FALSE)</f>
@@ -8605,7 +8581,7 @@
         <v>1027</v>
       </c>
       <c r="B12" t="s">
-        <v>1072</v>
+        <v>1035</v>
       </c>
       <c r="C12" t="str">
         <f>VLOOKUP("Cisco Nexus 1110-X A",Nexus_5548_A,2,FALSE)</f>
@@ -8617,7 +8593,7 @@
         <v>1027</v>
       </c>
       <c r="B13" t="s">
-        <v>1071</v>
+        <v>1036</v>
       </c>
       <c r="C13" t="str">
         <f>VLOOKUP("Cisco Nexus 1110-X B",Nexus_5548_A,2,FALSE)</f>
@@ -8629,7 +8605,7 @@
         <v>1028</v>
       </c>
       <c r="B14" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C14" t="str">
         <f>VLOOKUP("NetApp Controller A",Nexus_5548_B,2,FALSE)</f>
@@ -8641,7 +8617,7 @@
         <v>1028</v>
       </c>
       <c r="B15" t="s">
-        <v>1029</v>
+        <v>1032</v>
       </c>
       <c r="C15" t="str">
         <f>VLOOKUP("NetApp Controller B",Nexus_5548_B,2,FALSE)</f>
@@ -8653,7 +8629,7 @@
         <v>1028</v>
       </c>
       <c r="B16" t="s">
-        <v>1032</v>
+        <v>1061</v>
       </c>
       <c r="C16" t="str">
         <f>VLOOKUP("NetApp Controller A (cluster)",Nexus_5548_B,2,FALSE)</f>
@@ -8665,7 +8641,7 @@
         <v>1028</v>
       </c>
       <c r="B17" t="s">
-        <v>1031</v>
+        <v>1062</v>
       </c>
       <c r="C17" t="str">
         <f>VLOOKUP("NetApp Controller B (cluster)",Nexus_5548_B,2,FALSE)</f>
@@ -8677,7 +8653,7 @@
         <v>1028</v>
       </c>
       <c r="B18" t="s">
-        <v>1033</v>
+        <v>1063</v>
       </c>
       <c r="C18" t="str">
         <f>VLOOKUP("Cisco Nexus 5548 A (1)",Nexus_5548_B,2,FALSE)</f>
@@ -8689,7 +8665,7 @@
         <v>1028</v>
       </c>
       <c r="B19" t="s">
-        <v>1034</v>
+        <v>1064</v>
       </c>
       <c r="C19" t="str">
         <f>VLOOKUP("Cisco Nexus 5548 A (2)",Nexus_5548_B,2,FALSE)</f>
@@ -8701,7 +8677,7 @@
         <v>1028</v>
       </c>
       <c r="B20" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C20" t="str">
         <f>VLOOKUP("Cisco UCS Fabric Interconnect A",Nexus_5548_B,2,FALSE)</f>
@@ -8713,7 +8689,7 @@
         <v>1028</v>
       </c>
       <c r="B21" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C21" t="str">
         <f>VLOOKUP("Cisco UCS Fabric Interconnect B",Nexus_5548_B,2,FALSE)</f>
@@ -8725,7 +8701,7 @@
         <v>1028</v>
       </c>
       <c r="B22" t="s">
-        <v>1039</v>
+        <v>1067</v>
       </c>
       <c r="C22" t="str">
         <f>VLOOKUP("Cisco UCS Fabric Interconnect B (FAB B1)",Nexus_5548_B,2,FALSE)</f>
@@ -8737,7 +8713,7 @@
         <v>1028</v>
       </c>
       <c r="B23" t="s">
-        <v>1040</v>
+        <v>1068</v>
       </c>
       <c r="C23" t="str">
         <f>VLOOKUP("Cisco UCS Fabric Interconnect B (FAB B2)",Nexus_5548_B,2,FALSE)</f>
@@ -8749,7 +8725,7 @@
         <v>1028</v>
       </c>
       <c r="B24" t="s">
-        <v>1072</v>
+        <v>1035</v>
       </c>
       <c r="C24" t="str">
         <f>VLOOKUP("Cisco Nexus 1110-X A",Nexus_5548_B,2,FALSE)</f>
@@ -8761,7 +8737,7 @@
         <v>1028</v>
       </c>
       <c r="B25" t="s">
-        <v>1071</v>
+        <v>1036</v>
       </c>
       <c r="C25" t="str">
         <f>VLOOKUP("Cisco Nexus 1110-X B",Nexus_5548_B,2,FALSE)</f>
@@ -8770,10 +8746,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="B26" t="s">
-        <v>1049</v>
+        <v>1069</v>
       </c>
       <c r="C26" t="str">
         <f>VLOOKUP("GbE management switch",NetApp_A,2,FALSE)</f>
@@ -8782,10 +8758,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="B27" t="s">
-        <v>1047</v>
+        <v>1070</v>
       </c>
       <c r="C27" t="str">
         <f>VLOOKUP("NetApp Controller B (1)",NetApp_A,2,FALSE)</f>
@@ -8794,10 +8770,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="B28" t="s">
-        <v>1046</v>
+        <v>1071</v>
       </c>
       <c r="C28" t="str">
         <f>VLOOKUP("NetApp Controller B (2)",NetApp_A,2,FALSE)</f>
@@ -8806,10 +8782,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="B29" t="s">
-        <v>1048</v>
+        <v>1072</v>
       </c>
       <c r="C29" t="str">
         <f>VLOOKUP("SAS shelves",NetApp_A,2,FALSE)</f>
@@ -8818,10 +8794,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="B30" t="s">
-        <v>1045</v>
+        <v>1073</v>
       </c>
       <c r="C30" t="str">
         <f>VLOOKUP("Nexus 5548 A (cluster)",NetApp_A,2,FALSE)</f>
@@ -8830,10 +8806,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="B31" t="s">
-        <v>1044</v>
+        <v>1074</v>
       </c>
       <c r="C31" t="str">
         <f>VLOOKUP("Nexus 5548 B (cluster)",NetApp_A,2,FALSE)</f>
@@ -8842,10 +8818,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="B32" t="s">
-        <v>1051</v>
+        <v>1027</v>
       </c>
       <c r="C32" t="str">
         <f>VLOOKUP("Nexus 5548 A",NetApp_A,2,FALSE)</f>
@@ -8854,10 +8830,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="B33" t="s">
-        <v>1050</v>
+        <v>1028</v>
       </c>
       <c r="C33" t="str">
         <f>VLOOKUP("Nexus 5548 B",NetApp_A,2,FALSE)</f>
@@ -8866,10 +8842,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1052</v>
+        <v>1032</v>
       </c>
       <c r="B34" t="s">
-        <v>1049</v>
+        <v>1069</v>
       </c>
       <c r="C34" t="str">
         <f>VLOOKUP("GbE management switch",NetApp_B,2,FALSE)</f>
@@ -8878,10 +8854,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1052</v>
+        <v>1032</v>
       </c>
       <c r="B35" t="s">
-        <v>1053</v>
+        <v>1075</v>
       </c>
       <c r="C35" t="str">
         <f>VLOOKUP("NetApp Controller A (1)",NetApp_B,2,FALSE)</f>
@@ -8890,10 +8866,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1052</v>
+        <v>1032</v>
       </c>
       <c r="B36" t="s">
-        <v>1054</v>
+        <v>1076</v>
       </c>
       <c r="C36" t="str">
         <f>VLOOKUP("NetApp Controller A (2)",NetApp_B,2,FALSE)</f>
@@ -8902,10 +8878,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1052</v>
+        <v>1032</v>
       </c>
       <c r="B37" t="s">
-        <v>1048</v>
+        <v>1072</v>
       </c>
       <c r="C37" t="str">
         <f>VLOOKUP("SAS shelves",NetApp_B,2,FALSE)</f>
@@ -8914,10 +8890,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1052</v>
+        <v>1032</v>
       </c>
       <c r="B38" t="s">
-        <v>1045</v>
+        <v>1073</v>
       </c>
       <c r="C38" t="str">
         <f>VLOOKUP("Nexus 5548 A (cluster)",NetApp_B,2,FALSE)</f>
@@ -8926,10 +8902,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1052</v>
+        <v>1032</v>
       </c>
       <c r="B39" t="s">
-        <v>1044</v>
+        <v>1074</v>
       </c>
       <c r="C39" t="str">
         <f>VLOOKUP("Nexus 5548 B (cluster)",NetApp_B,2,FALSE)</f>
@@ -8938,10 +8914,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1052</v>
+        <v>1032</v>
       </c>
       <c r="B40" t="s">
-        <v>1051</v>
+        <v>1027</v>
       </c>
       <c r="C40" t="str">
         <f>VLOOKUP("Nexus 5548 A",NetApp_B,2,FALSE)</f>
@@ -8950,10 +8926,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1052</v>
+        <v>1032</v>
       </c>
       <c r="B41" t="s">
-        <v>1050</v>
+        <v>1028</v>
       </c>
       <c r="C41" t="str">
         <f>VLOOKUP("Nexus 5548 B",NetApp_B,2,FALSE)</f>
@@ -8962,10 +8938,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="B42" t="s">
-        <v>1056</v>
+        <v>1077</v>
       </c>
       <c r="C42" t="str">
         <f>VLOOKUP("Chassis 1 FEX A (1)",UCS_FI_A,2,FALSE)</f>
@@ -8974,10 +8950,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="B43" t="s">
-        <v>1059</v>
+        <v>1078</v>
       </c>
       <c r="C43" t="str">
         <f>VLOOKUP("Chassis 1 FEX A (2)",UCS_FI_A,2,FALSE)</f>
@@ -8986,10 +8962,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="B44" t="s">
-        <v>1058</v>
+        <v>1079</v>
       </c>
       <c r="C44" t="str">
         <f>VLOOKUP("Chassis 1 FEX A (3)",UCS_FI_A,2,FALSE)</f>
@@ -8998,10 +8974,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="B45" t="s">
-        <v>1057</v>
+        <v>1080</v>
       </c>
       <c r="C45" t="str">
         <f>VLOOKUP("Chassis 1 FEX A (4)",UCS_FI_A,2,FALSE)</f>
@@ -9010,10 +8986,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="B46" t="s">
-        <v>1051</v>
+        <v>1027</v>
       </c>
       <c r="C46" t="str">
         <f>VLOOKUP("Nexus 5548 A",UCS_FI_A,2,FALSE)</f>
@@ -9022,10 +8998,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="B47" t="s">
-        <v>1050</v>
+        <v>1028</v>
       </c>
       <c r="C47" t="str">
         <f>VLOOKUP("Nexus 5548 B",UCS_FI_A,2,FALSE)</f>
@@ -9034,10 +9010,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="B48" t="s">
-        <v>1060</v>
+        <v>1081</v>
       </c>
       <c r="C48" t="str">
         <f>VLOOKUP("Nexus 5548 A (FAB A1)",UCS_FI_A,2,FALSE)</f>
@@ -9046,10 +9022,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="B49" t="s">
-        <v>1061</v>
+        <v>1082</v>
       </c>
       <c r="C49" t="str">
         <f>VLOOKUP("Nexus 5548 A (FAB A2)",UCS_FI_A,2,FALSE)</f>
@@ -9058,10 +9034,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
       <c r="B50" t="s">
-        <v>1063</v>
+        <v>1083</v>
       </c>
       <c r="C50" t="str">
         <f>VLOOKUP("Chassis 1 FEX B (1)",UCS_FI_B,2,FALSE)</f>
@@ -9070,10 +9046,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
       <c r="B51" t="s">
-        <v>1064</v>
+        <v>1084</v>
       </c>
       <c r="C51" t="str">
         <f>VLOOKUP("Chassis 1 FEX B (2)",UCS_FI_B,2,FALSE)</f>
@@ -9082,10 +9058,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
       <c r="B52" t="s">
-        <v>1065</v>
+        <v>1085</v>
       </c>
       <c r="C52" t="str">
         <f>VLOOKUP("Chassis 1 FEX B (3)",UCS_FI_B,2,FALSE)</f>
@@ -9094,10 +9070,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
       <c r="B53" t="s">
-        <v>1066</v>
+        <v>1086</v>
       </c>
       <c r="C53" t="str">
         <f>VLOOKUP("Chassis 1 FEX B (4)",UCS_FI_B,2,FALSE)</f>
@@ -9106,10 +9082,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
       <c r="B54" t="s">
-        <v>1051</v>
+        <v>1027</v>
       </c>
       <c r="C54" t="str">
         <f>VLOOKUP("Nexus 5548 A",UCS_FI_B,2,FALSE)</f>
@@ -9118,10 +9094,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
       <c r="B55" t="s">
-        <v>1050</v>
+        <v>1028</v>
       </c>
       <c r="C55" t="str">
         <f>VLOOKUP("Nexus 5548 B",UCS_FI_B,2,FALSE)</f>
@@ -9130,10 +9106,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
       <c r="B56" t="s">
-        <v>1067</v>
+        <v>1087</v>
       </c>
       <c r="C56" t="str">
         <f>VLOOKUP("Nexus 5548 B (FAB B1)",UCS_FI_B,2,FALSE)</f>
@@ -9142,10 +9118,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
       <c r="B57" t="s">
-        <v>1068</v>
+        <v>1088</v>
       </c>
       <c r="C57" t="str">
         <f>VLOOKUP("Nexus 5548 B (FAB B2)",UCS_FI_B,2,FALSE)</f>
@@ -9154,10 +9130,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1069</v>
+        <v>1035</v>
       </c>
       <c r="B58" t="s">
-        <v>1051</v>
+        <v>1027</v>
       </c>
       <c r="C58" t="str">
         <f>VLOOKUP("Cisco Nexus 5548 A",Nexus_1000V_A,2,FALSE)</f>
@@ -9166,10 +9142,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1069</v>
+        <v>1035</v>
       </c>
       <c r="B59" t="s">
-        <v>1050</v>
+        <v>1028</v>
       </c>
       <c r="C59" t="str">
         <f>VLOOKUP("Cisco Nexus 5548 B",Nexus_1000V_A,2,FALSE)</f>
@@ -9178,10 +9154,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1070</v>
+        <v>1036</v>
       </c>
       <c r="B60" t="s">
-        <v>1051</v>
+        <v>1027</v>
       </c>
       <c r="C60" t="str">
         <f>VLOOKUP("Cisco Nexus 5548 A",Nexus_1000v_B,2,FALSE)</f>
@@ -9190,10 +9166,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1070</v>
+        <v>1036</v>
       </c>
       <c r="B61" t="s">
-        <v>1050</v>
+        <v>1028</v>
       </c>
       <c r="C61" t="str">
         <f>VLOOKUP("Cisco Nexus 5548 B",Nexus_1000v_B,2,FALSE)</f>
@@ -11460,8 +11436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76:E77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11568,7 +11544,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
-        <v>1090</v>
+        <v>1054</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>251</v>
@@ -11584,7 +11560,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="2" t="s">
-        <v>1089</v>
+        <v>1053</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>250</v>
@@ -11632,7 +11608,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="2" t="s">
-        <v>1088</v>
+        <v>1052</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>253</v>
@@ -11648,7 +11624,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
-        <v>1087</v>
+        <v>1051</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>252</v>
@@ -11777,7 +11753,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="2" t="s">
-        <v>1086</v>
+        <v>1050</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>251</v>
@@ -11793,7 +11769,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="2" t="s">
-        <v>1085</v>
+        <v>1049</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>250</v>
@@ -11841,7 +11817,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="2" t="s">
-        <v>1084</v>
+        <v>1048</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>253</v>
@@ -11857,7 +11833,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="2" t="s">
-        <v>1083</v>
+        <v>1047</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>252</v>
@@ -11978,7 +11954,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="2" t="s">
-        <v>1082</v>
+        <v>1046</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>267</v>
@@ -11994,7 +11970,7 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="2" t="s">
-        <v>1081</v>
+        <v>1045</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>268</v>
@@ -12025,7 +12001,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="2" t="s">
-        <v>1042</v>
+        <v>1030</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>262</v>
@@ -12041,7 +12017,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="2" t="s">
-        <v>1043</v>
+        <v>1031</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>131</v>
@@ -12121,7 +12097,7 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="25"/>
       <c r="B42" s="2" t="s">
-        <v>1080</v>
+        <v>1044</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>267</v>
@@ -12137,7 +12113,7 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="25"/>
       <c r="B43" s="2" t="s">
-        <v>1079</v>
+        <v>1043</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>268</v>
@@ -12168,7 +12144,7 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="2" t="s">
-        <v>1042</v>
+        <v>1030</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>262</v>
@@ -12184,7 +12160,7 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="2" t="s">
-        <v>1043</v>
+        <v>1031</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>131</v>
@@ -12260,7 +12236,7 @@
         <v>149</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>1076</v>
+        <v>1040</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>128</v>
@@ -12275,7 +12251,7 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="2" t="s">
-        <v>1075</v>
+        <v>1039</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>132</v>
@@ -12290,7 +12266,7 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="2" t="s">
-        <v>1074</v>
+        <v>1038</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>153</v>
@@ -12305,7 +12281,7 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="2" t="s">
-        <v>1073</v>
+        <v>1037</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>154</v>
@@ -12352,7 +12328,7 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="23"/>
       <c r="B57" s="2" t="s">
-        <v>1077</v>
+        <v>1041</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>253</v>
@@ -12368,7 +12344,7 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
       <c r="B58" s="2" t="s">
-        <v>1078</v>
+        <v>1042</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>252</v>
@@ -12433,7 +12409,7 @@
         <v>149</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>1093</v>
+        <v>1057</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>128</v>
@@ -12448,7 +12424,7 @@
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="23"/>
       <c r="B63" s="2" t="s">
-        <v>1094</v>
+        <v>1058</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>132</v>
@@ -12463,7 +12439,7 @@
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
       <c r="B64" s="2" t="s">
-        <v>1095</v>
+        <v>1059</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>153</v>
@@ -12478,7 +12454,7 @@
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="23"/>
       <c r="B65" s="2" t="s">
-        <v>1096</v>
+        <v>1060</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>154</v>
@@ -12525,7 +12501,7 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="23"/>
       <c r="B68" s="2" t="s">
-        <v>1092</v>
+        <v>1056</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>253</v>
@@ -12541,7 +12517,7 @@
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="23"/>
       <c r="B69" s="2" t="s">
-        <v>1091</v>
+        <v>1055</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>252</v>

</xml_diff>